<commit_message>
Added Zev's simulation with 100k voters
</commit_message>
<xml_diff>
--- a/LargeVoterImplementation.xlsx
+++ b/LargeVoterImplementation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Josh/Desktop/Math and Democracy/VotingSystems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B10DFE4-F02F-F943-B0F6-E78BF5C2D31F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96E8E30-2A88-514E-9455-CD1B0136F574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -390,11 +390,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" zoomScale="162" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="8" width="7.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1">

</xml_diff>

<commit_message>
Implimented the comparitive heatmap
</commit_message>
<xml_diff>
--- a/LargeVoterImplementation.xlsx
+++ b/LargeVoterImplementation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Josh/Desktop/Math and Democracy/VotingSystems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96E8E30-2A88-514E-9455-CD1B0136F574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944ACD38-1F17-604A-8B93-46514542DFB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,6 +28,10 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -390,8 +394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="W25" sqref="A23:W25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -919,6 +923,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:H20">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24:V24">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>